<commit_message>
Updated DB Importer so it can use google sheet directly
</commit_message>
<xml_diff>
--- a/ImportSpreadSheet.xlsx
+++ b/ImportSpreadSheet.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="150">
   <si>
     <t>id</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>object_name</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Ladder</t>
   </si>
   <si>
     <t>Climb-down</t>
@@ -929,43 +935,43 @@
         <v>23</v>
       </c>
       <c r="C4" s="1">
-        <v>31030.0</v>
+        <v>24373.0</v>
       </c>
       <c r="D4" s="1">
-        <v>2112.0</v>
+        <v>24369.0</v>
       </c>
       <c r="E4" s="1">
-        <v>3046.0</v>
+        <v>2815.0</v>
       </c>
       <c r="F4" s="1">
-        <v>9757.0</v>
+        <v>3182.0</v>
       </c>
       <c r="G4" s="1">
         <v>0.0</v>
       </c>
       <c r="H4" s="1">
-        <v>3046.0</v>
+        <v>2816.0</v>
       </c>
       <c r="I4" s="1">
-        <v>9756.0</v>
+        <v>3182.0</v>
       </c>
       <c r="J4" s="1">
         <v>0.0</v>
       </c>
       <c r="K4" s="1">
-        <v>3046.0</v>
+        <v>2815.0</v>
       </c>
       <c r="L4" s="1">
-        <v>9756.0</v>
+        <v>3182.0</v>
       </c>
       <c r="M4" s="1">
         <v>0.0</v>
       </c>
       <c r="N4" s="1">
-        <v>3046.0</v>
+        <v>2816.0</v>
       </c>
       <c r="O4" s="1">
-        <v>9757.0</v>
+        <v>3182.0</v>
       </c>
       <c r="P4" s="1">
         <v>0.0</v>
@@ -985,43 +991,43 @@
         <v>21</v>
       </c>
       <c r="C5" s="1">
-        <v>31030.0</v>
+        <v>24373.0</v>
       </c>
       <c r="D5" s="1">
-        <v>2112.0</v>
+        <v>24369.0</v>
       </c>
       <c r="E5" s="1">
-        <v>3046.0</v>
+        <v>2815.0</v>
       </c>
       <c r="F5" s="1">
-        <v>9757.0</v>
+        <v>3182.0</v>
       </c>
       <c r="G5" s="1">
         <v>0.0</v>
       </c>
       <c r="H5" s="1">
-        <v>3046.0</v>
+        <v>2816.0</v>
       </c>
       <c r="I5" s="1">
-        <v>9756.0</v>
+        <v>3182.0</v>
       </c>
       <c r="J5" s="1">
         <v>0.0</v>
       </c>
       <c r="K5" s="1">
-        <v>3046.0</v>
+        <v>2815.0</v>
       </c>
       <c r="L5" s="1">
-        <v>9756.0</v>
+        <v>3182.0</v>
       </c>
       <c r="M5" s="1">
         <v>0.0</v>
       </c>
       <c r="N5" s="1">
-        <v>3046.0</v>
+        <v>2816.0</v>
       </c>
       <c r="O5" s="1">
-        <v>9757.0</v>
+        <v>3182.0</v>
       </c>
       <c r="P5" s="1">
         <v>0.0</v>
@@ -1035,55 +1041,55 @@
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="1">
-        <v>24373.0</v>
+        <v>-1.0</v>
       </c>
       <c r="D6" s="1">
-        <v>24369.0</v>
+        <v>65346.0</v>
       </c>
       <c r="E6" s="1">
-        <v>2815.0</v>
+        <v>3158.0</v>
       </c>
       <c r="F6" s="1">
-        <v>3182.0</v>
+        <v>3951.0</v>
       </c>
       <c r="G6" s="1">
         <v>0.0</v>
       </c>
       <c r="H6" s="1">
-        <v>2816.0</v>
+        <v>3158.0</v>
       </c>
       <c r="I6" s="1">
-        <v>3182.0</v>
+        <v>3951.0</v>
       </c>
       <c r="J6" s="1">
         <v>0.0</v>
       </c>
       <c r="K6" s="1">
-        <v>2815.0</v>
+        <v>3158.0</v>
       </c>
       <c r="L6" s="1">
-        <v>3182.0</v>
+        <v>3950.0</v>
       </c>
       <c r="M6" s="1">
         <v>0.0</v>
       </c>
       <c r="N6" s="1">
-        <v>2816.0</v>
+        <v>3158.0</v>
       </c>
       <c r="O6" s="1">
-        <v>3182.0</v>
+        <v>3951.0</v>
       </c>
       <c r="P6" s="1">
         <v>0.0</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="R6" s="1">
         <v>600.0</v>
@@ -1091,10 +1097,10 @@
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1">
         <v>-1.0</v>
@@ -1142,62 +1148,6 @@
         <v>24</v>
       </c>
       <c r="R7" s="1">
-        <v>600.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="1">
-        <v>-1.0</v>
-      </c>
-      <c r="D8" s="1">
-        <v>65346.0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>3158.0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>3951.0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H8" s="1">
-        <v>3158.0</v>
-      </c>
-      <c r="I8" s="1">
-        <v>3951.0</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="K8" s="1">
-        <v>3158.0</v>
-      </c>
-      <c r="L8" s="1">
-        <v>3950.0</v>
-      </c>
-      <c r="M8" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="N8" s="1">
-        <v>3158.0</v>
-      </c>
-      <c r="O8" s="1">
-        <v>3951.0</v>
-      </c>
-      <c r="P8" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="R8" s="1">
         <v>600.0</v>
       </c>
     </row>
@@ -1684,13 +1634,13 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2113.0</v>
+        <v>50</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F2" s="1">
         <v>3017.0</v>
@@ -1740,7 +1690,7 @@
         <v>1814.0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F3" s="1">
         <v>3153.0</v>
@@ -1774,6 +1724,106 @@
       </c>
       <c r="P3" s="1">
         <v>20.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2112.0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3045.0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>3047.0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>9755.0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>9756.0</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>3045.0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>3047.0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>9757.0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>9758.0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>20.0</v>
+      </c>
+      <c r="T4" s="1">
+        <v>30.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2112.0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3045.0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3047.0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>9757.0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>9758.0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>3045.0</v>
+      </c>
+      <c r="L5" s="1">
+        <v>3047.0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>9755.0</v>
+      </c>
+      <c r="N5" s="1">
+        <v>9756.0</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="P5" s="1">
+        <v>20.0</v>
+      </c>
+      <c r="T5" s="1">
+        <v>30.0</v>
       </c>
     </row>
   </sheetData>
@@ -1796,13 +1846,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>33</v>
@@ -1825,7 +1875,7 @@
         <v>3.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C2" s="1">
         <v>3297.0</v>
@@ -1848,7 +1898,7 @@
         <v>4.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1">
         <v>5431.0</v>
@@ -1871,7 +1921,7 @@
         <v>5.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C4" s="1">
         <v>2634.0</v>
@@ -1894,7 +1944,7 @@
         <v>6.0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C5" s="1">
         <v>2474.0</v>
@@ -1917,7 +1967,7 @@
         <v>7.0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C6" s="1">
         <v>3214.0</v>
@@ -1937,7 +1987,7 @@
         <v>8.0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C7" s="1">
         <v>2899.0</v>
@@ -1960,7 +2010,7 @@
         <v>9.0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C8" s="1">
         <v>3517.0</v>
@@ -1983,7 +2033,7 @@
         <v>10.0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C9" s="1">
         <v>2811.0</v>
@@ -2006,7 +2056,7 @@
         <v>11.0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C10" s="1">
         <v>3105.0</v>
@@ -2029,7 +2079,7 @@
         <v>12.0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C11" s="1">
         <v>2366.0</v>
@@ -2052,7 +2102,7 @@
         <v>13.0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C12" s="1">
         <v>3067.0</v>
@@ -2075,7 +2125,7 @@
         <v>14.0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C13" s="1">
         <v>2967.0</v>
@@ -2098,7 +2148,7 @@
         <v>15.0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C14" s="1">
         <v>3298.0</v>
@@ -2121,7 +2171,7 @@
         <v>16.0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C15" s="1">
         <v>2712.0</v>
@@ -2144,7 +2194,7 @@
         <v>17.0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C16" s="1">
         <v>2761.0</v>
@@ -2167,7 +2217,7 @@
         <v>18.0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C17" s="1">
         <v>2085.0</v>
@@ -2187,7 +2237,7 @@
         <v>19.0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C18" s="1">
         <v>3233.0</v>
@@ -2210,7 +2260,7 @@
         <v>20.0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C19" s="1">
         <v>3216.0</v>
@@ -2233,7 +2283,7 @@
         <v>21.0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C20" s="1">
         <v>2532.0</v>
@@ -2256,7 +2306,7 @@
         <v>22.0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C21" s="1">
         <v>3011.0</v>
@@ -2279,7 +2329,7 @@
         <v>23.0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C22" s="1">
         <v>2208.0</v>
@@ -2302,7 +2352,7 @@
         <v>24.0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C23" s="1">
         <v>2689.0</v>
@@ -2325,7 +2375,7 @@
         <v>25.0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C24" s="1">
         <v>2878.0</v>
@@ -2348,7 +2398,7 @@
         <v>26.0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C25" s="1">
         <v>2254.0</v>
@@ -2371,7 +2421,7 @@
         <v>27.0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C26" s="1">
         <v>1084.0</v>
@@ -2394,7 +2444,7 @@
         <v>28.0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C27" s="1">
         <v>3214.0</v>
@@ -2417,7 +2467,7 @@
         <v>29.0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C28" s="1">
         <v>3143.0</v>
@@ -2440,7 +2490,7 @@
         <v>30.0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C29" s="1">
         <v>2529.0</v>
@@ -2481,16 +2531,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2">
@@ -2498,16 +2548,16 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D2" s="1">
         <v>30.0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3">
@@ -2515,16 +2565,16 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D3" s="1">
         <v>1.0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4">
@@ -2532,16 +2582,16 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="5">
@@ -2549,16 +2599,16 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D5" s="1">
         <v>1.0</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6">
@@ -2566,16 +2616,16 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D6" s="1">
         <v>1.0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7">
@@ -2583,16 +2633,16 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D7" s="1">
         <v>1.0</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8">
@@ -2600,16 +2650,16 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D8" s="1">
         <v>1.0</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9">
@@ -2617,16 +2667,16 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D9" s="1">
         <v>1.0</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10">
@@ -2634,16 +2684,16 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D10" s="1">
         <v>1.0</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11">
@@ -2651,16 +2701,16 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D11" s="1">
         <v>1.0</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12">
@@ -2668,16 +2718,16 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D12" s="1">
         <v>1.0</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13">
@@ -2685,16 +2735,16 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D13" s="1">
         <v>1.0</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14">
@@ -2702,16 +2752,16 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D14" s="1">
         <v>1.0</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15">
@@ -2719,16 +2769,16 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D15" s="1">
         <v>1.0</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16">
@@ -2736,16 +2786,16 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D16" s="1">
         <v>1.0</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17">
@@ -2753,16 +2803,16 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D17" s="1">
         <v>1.0</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18">
@@ -2770,16 +2820,16 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D18" s="1">
         <v>1.0</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19">
@@ -2787,16 +2837,16 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D19" s="1">
         <v>1.0</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20">
@@ -2804,16 +2854,16 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D20" s="1">
         <v>1.0</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21">
@@ -2821,16 +2871,16 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D21" s="1">
         <v>1.0</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22">
@@ -2838,16 +2888,16 @@
         <v>21.0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D22" s="1">
         <v>1.0</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23">
@@ -2855,16 +2905,16 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D23" s="1">
         <v>1.0</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24">
@@ -2872,7 +2922,7 @@
         <v>23.0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25">
@@ -2880,16 +2930,16 @@
         <v>24.0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D25" s="1">
         <v>1.0</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26">
@@ -2897,16 +2947,16 @@
         <v>25.0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D26" s="1">
         <v>1.0</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27">
@@ -2914,16 +2964,16 @@
         <v>26.0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D27" s="1">
         <v>1.0</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28">
@@ -2931,16 +2981,16 @@
         <v>27.0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D28" s="1">
         <v>1.0</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29">
@@ -2948,16 +2998,16 @@
         <v>28.0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D29" s="1">
         <v>1.0</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30">
@@ -2965,16 +3015,16 @@
         <v>29.0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D30" s="1">
         <v>1.0</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31">
@@ -2982,16 +3032,16 @@
         <v>30.0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D31" s="1">
         <v>60.0</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>